<commit_message>
created script to create results
</commit_message>
<xml_diff>
--- a/data/lookup_table.xlsx
+++ b/data/lookup_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominic\DataspellProjects\bt_data_analysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominic\DataspellProjects\ba_data_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D366482-902E-4C41-AF00-1A4B9AF4ED6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C8747C-BB00-4280-97A7-08AB0E3C54D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11580" xr2:uid="{97050E6A-45AA-4CF0-95A5-432DAC50CC67}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{97050E6A-45AA-4CF0-95A5-432DAC50CC67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,22 +36,103 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>LinkId</t>
   </si>
   <si>
     <t>NumAnswers</t>
+  </si>
+  <si>
+    <t>zero_index</t>
+  </si>
+  <si>
+    <t>one_index</t>
+  </si>
+  <si>
+    <t>na_index</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Wurden Ihnen die möglichen Nebenwirkungen der Behandlung(en) in verständlicher Weise erklärt?</t>
+  </si>
+  <si>
+    <t>Hat man Sie auch über Nebenwirkungen informiert, die später und nicht nur direkt im Anschluss an die Behandlung auftreten können?</t>
+  </si>
+  <si>
+    <t>Wurden Sie in die Entscheidungen bezüglich Ihrer Behandlungen in gewünschtem Umfang einbezogen?</t>
+  </si>
+  <si>
+    <t>Waren Ihre Familie oder nahestehende Personen im von Ihnen gewünschten Umfang in die Entscheidungen zu Ihren Behandlungen einbezogen?</t>
+  </si>
+  <si>
+    <t>Wurden Ihre Lebensgewohnheiten und Ihre familiäre und/oder berufliche Situation bei den Entscheidungen zu Ihren Behandlungen berücksichtigt?</t>
+  </si>
+  <si>
+    <t>Hat man mit Ihnen darüber gesprochen oder Ihnen Informationen dazu gegeben, welche Auswirkungen die Krebserkrankung auf Ihren Alltag hat (zum Beispiel auf Ihrer Arbeit, auf Ihre Freizeit)?</t>
+  </si>
+  <si>
+    <t>Hat man Ihnen ausreichend praktische Ratschläge gegeben und/oder Unterstützung angeboten, um mit den Langzeitfolgen der Krebserkrankung oder der Behandlungen um-zugehen (zum Beispiel Müdigkeit, Schmerzen, Angst)?</t>
+  </si>
+  <si>
+    <t>Hatten Sie am Ende der Behandlungen alle nötigen Informationen zur Nachsorge?</t>
+  </si>
+  <si>
+    <t>Stehen Sie in regelmässigem Kontakt mit einer Bezugsperson (zum Beispiel: Arzt/Ärztin, Pflegefach-person, Sozialarbeiter:in) wegen der Nachsorge?</t>
+  </si>
+  <si>
+    <t>Wenn ja, mit welcher?</t>
+  </si>
+  <si>
+    <t>Hat man Ihnen Informationen zu Unterstützungs- oder Selbsthilfegruppen für Krebsbetroffene gegeben?</t>
+  </si>
+  <si>
+    <t>Hat man Ihnen Informationen zu Hilfs- und Unterstützungsangeboten gegeben, um Ihnen zu helfen, mit Ihren Gefühlen umzugehen (zum Beispiel Stress, Angst, Traurigkeit)?</t>
+  </si>
+  <si>
+    <t>Hat man Ihnen Informationen dazu gegeben, wie Sie finanzielle Unterstützung oder Leistungen erhalten können, auf die Sie möglicherweise Anspruch haben?</t>
+  </si>
+  <si>
+    <t>Haben die verschiedenen Personen, die Sie behandelt und betreut haben (wie Ihr:e Hausarzt/-ärztin, Onkologe/-in, die Ärzteschaft und Pflegefachpersonen im Spital, Spitex) gut zusammengearbeitet, um Ihnen die bestmögliche Versorgung zu bieten?</t>
+  </si>
+  <si>
+    <t>Hat man Ihnen einen Behandlungsplan gegeben? (Dabei handelt es sich um ein schriftliches Dokument, in dem Ihre Bedürfnisse und Ziele in Bezug auf die Behandlung der Krebserkrankung dargestellt sind</t>
+  </si>
+  <si>
+    <t>Kam es im Lauf Ihrer Behandlung vor, dass Testergebnisse oder Ihre Krankenakte nicht rechtzeitig zum Behandlungstermin verfügbar waren?</t>
+  </si>
+  <si>
+    <t>Kam es im Lauf Ihrer Behandlung vor, dass man Ihnen verwirrende oder widersprüchliche Informationen zu Ihrem Gesundheitszustand oder Ihren Behandlungen gegeben hat?</t>
+  </si>
+  <si>
+    <t>Hatten Sie während Ihrer Behandlung den Eindruck, dass Tests oder andere Analysen unnötig wiederholt wurden?</t>
+  </si>
+  <si>
+    <t>Wie schätzen Sie Ihre Behandlung und Betreuung insgesamt ein?</t>
+  </si>
+  <si>
+    <t>Haben Sie Verständnisprobleme, wenn Sie eine schriftliche Information zu einer medizinischen Behandlung oder zu Ihrem Gesundheitszustand erhalten?</t>
+  </si>
+  <si>
+    <t>Wie möchten Sie generell, dass medizinische Entscheidungen über Krebsbehandlungen getroffen werden?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -76,11 +157,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -96,7 +178,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -412,128 +494,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4E5715-436F-4A0A-B979-15F713F46845}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F1" sqref="F1:F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A17">
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A18">
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A19">
+      <c r="B18" s="1">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="B19" s="1">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>